<commit_message>
Added rates from dad
</commit_message>
<xml_diff>
--- a/RatesBrochure.xlsx
+++ b/RatesBrochure.xlsx
@@ -1169,12 +1169,12 @@
   <dimension ref="A1:E183"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>

</xml_diff>